<commit_message>
Update pricing models, init_db service, and Excel data with new pricing configurations
</commit_message>
<xml_diff>
--- a/static/istanbul_transfer.xlsx
+++ b/static/istanbul_transfer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,19 +496,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>İstanbul Havalimanı (IST)</t>
+          <t>Beşiktaş</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sabiha Gökçen Havalimanı (SAW)</t>
+          <t>Kadıköy</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -524,6 +524,82 @@
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>İstanbul Havalimanı (IST)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Sabiha Gökçen Havalimanı (SAW)</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>12</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>İstanbul Havalimanı (IST)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Sultanahmet, Fatih</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2077</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2290</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2885</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2127</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Rakipten 50 TL ucuz (istanbulshuttleport.com)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>